<commit_message>
Add human-readable pipetting output
</commit_message>
<xml_diff>
--- a/examples/CAII-CBS/experiment.xlsx
+++ b/examples/CAII-CBS/experiment.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CaCl2*2H2O into PHIP 1</t>
+          <t>HEPES into PHIP 1</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1126,7 +1126,7 @@
         <v>0.01</v>
       </c>
       <c r="G16" t="n">
-        <v>1.291847692227915</v>
+        <v>9.332155665645574</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>CaCl2*2H2O into PHIP 1</t>
+          <t>HEPES into PHIP 1</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1175,7 +1175,7 @@
         <v>0.02</v>
       </c>
       <c r="G17" t="n">
-        <v>1.607687619682168</v>
+        <v>9.832728216575232</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1202,7 +1202,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CaCl2*2H2O into PHIP 1</t>
+          <t>HEPES into PHIP 1</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1224,7 +1224,7 @@
         <v>0.04000000000000001</v>
       </c>
       <c r="G18" t="n">
-        <v>2.157596873195582</v>
+        <v>10.70427564894001</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CaCl2*2H2O into PHIP 1</t>
+          <t>HEPES into PHIP 1</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1273,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>1.291847692227915</v>
+        <v>9.332155665645574</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>CaCl2*2H2O into PHIP 1</t>
+          <t>HEPES into PHIP 1</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>1.607687619682168</v>
+        <v>9.832728216575232</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CaCl2*2H2O into PHIP 1</t>
+          <t>HEPES into PHIP 1</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1371,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>2.157596873195582</v>
+        <v>10.70427564894001</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1398,29 +1398,29 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>HEPES into PHIP 1</t>
+          <t>final cleaning water titration</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Plates Quick.setup</t>
+          <t>Plates Clean.setup</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ChoderaHSA.inj</t>
+          <t>water5inj.inj</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Onesite</t>
+          <t>Control</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>9.332155665645574</v>
+        <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>HEPES into PHIP 1</t>
+          <t>final water into water test 1</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1457,19 +1457,19 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ChoderaHSA.inj</t>
+          <t>ChoderaWaterWater.inj</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Onesite</t>
+          <t>Control</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>9.832728216575232</v>
+        <v>0</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1485,300 +1485,6 @@
       <c r="K23" t="inlineStr">
         <is>
           <t>Plate1, C6</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>20191127a23.itc</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>HEPES into PHIP 1</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Plates Quick.setup</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>ChoderaHSA.inj</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Onesite</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>0.04000000000000001</v>
-      </c>
-      <c r="G24" t="n">
-        <v>10.70427564894001</v>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Plate1, E6</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>Plate1, F6</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>Plate1, E6</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>20191127a24.itc</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>HEPES into PHIP 1</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Plates Quick.setup</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>ChoderaHSA.inj</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Onesite</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" t="n">
-        <v>9.332155665645574</v>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>Plate1, G6</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>Plate1, H6</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>Plate1, G6</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>20191127a25.itc</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>HEPES into PHIP 1</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Plates Quick.setup</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>ChoderaHSA.inj</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Onesite</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" t="n">
-        <v>9.832728216575232</v>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>Plate1, A7</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>Plate1, B7</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>Plate1, A7</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>20191127a26.itc</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>HEPES into PHIP 1</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Plates Quick.setup</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>ChoderaHSA.inj</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Onesite</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" t="n">
-        <v>10.70427564894001</v>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Plate1, C7</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>Plate1, D7</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>Plate1, C7</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>20191127a27.itc</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>final cleaning water titration</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Plates Clean.setup</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>water5inj.inj</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Control</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Plate1, E7</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>Plate1, F7</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>Plate1, E7</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>20191127a28.itc</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>final water into water test 1</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Plates Quick.setup</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>ChoderaWaterWater.inj</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Control</t>
-        </is>
-      </c>
-      <c r="F29" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Plate1, G7</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>Plate1, H7</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>Plate1, G7</t>
         </is>
       </c>
     </row>

</xml_diff>